<commit_message>
feat: removed unused maps, modified templates files
</commit_message>
<xml_diff>
--- a/test/templates/simple.xlsx
+++ b/test/templates/simple.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{997F9485-0ED6-44E9-9D8A-0FD7DDDC88D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A2830A0-C2EE-4524-86C2-0AA6418140AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
+    <sheet name="#config" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>REPORT SUBJECT:</t>
   </si>
@@ -115,13 +116,58 @@
   </si>
   <si>
     <t>Total cost:</t>
+  </si>
+  <si>
+    <t>@Entities</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>@ListFilters</t>
+  </si>
+  <si>
+    <t>UI Label for parameter</t>
+  </si>
+  <si>
+    <t>Filter By</t>
+  </si>
+  <si>
+    <t>BusinessEntity</t>
+  </si>
+  <si>
+    <t>UIValueLabel</t>
+  </si>
+  <si>
+    <t>UIValueForFilter</t>
+  </si>
+  <si>
+    <t>Asset.id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>@RangeFilters</t>
+  </si>
+  <si>
+    <t>Jobs.StartDate</t>
+  </si>
+  <si>
+    <t>Jobs.CompletionDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +225,27 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -394,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -456,7 +523,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
@@ -469,6 +535,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G5:G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -799,7 +869,7 @@
     <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,7 +879,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="27">
+    <row r="2" spans="1:6" ht="27">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -821,7 +891,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -833,7 +903,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -845,34 +915,31 @@
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
@@ -882,10 +949,9 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
@@ -895,10 +961,9 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
@@ -908,10 +973,9 @@
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
@@ -921,10 +985,9 @@
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="12" t="s">
         <v>15</v>
       </c>
@@ -934,28 +997,25 @@
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="14"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
@@ -971,12 +1031,11 @@
       <c r="E15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="10" t="s">
         <v>23</v>
       </c>
@@ -993,22 +1052,20 @@
       <c r="E16" s="17">
         <v>10</v>
       </c>
-      <c r="F16" s="22" t="e">
+      <c r="F16" s="21" t="e">
         <f>E16*D16*24</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G16" s="21"/>
-    </row>
-    <row r="17" spans="1:7">
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="14"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75">
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
       <c r="A18" s="14"/>
       <c r="B18" s="13"/>
       <c r="C18" s="18" t="s">
@@ -1021,13 +1078,212 @@
       <c r="E18" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="25" t="e">
+      <c r="F18" s="24" t="e">
         <f>SUM(F16:F17)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G18" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA6A04C-FD9C-4CC0-9A8A-23F665EB3B7C}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="A10" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75">
+      <c r="A11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75">
+      <c r="A15" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75">
+      <c r="A16" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75">
+      <c r="A17" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75">
+      <c r="A18" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{1B2F9833-81C6-44C0-B10B-2478410F6C2C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove fix images sized
</commit_message>
<xml_diff>
--- a/test/templates/simple.xlsx
+++ b/test/templates/simple.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27321"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A2830A0-C2EE-4524-86C2-0AA6418140AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC14D4D-28CB-491F-8A73-18939993F31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -289,7 +289,7 @@
         <color rgb="FFCCCCCC"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
@@ -302,66 +302,6 @@
       </left>
       <right style="thin">
         <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FFCCCCCC"/>
@@ -457,88 +397,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,6 +528,105 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F52DFE-D03E-46E6-B5C0-E97283622024}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DB021ED9-CFE1-B73C-5371-7299953966C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7572375" y="76200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{610B0C8F-5991-4267-B99C-DC7FB8A71432}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{96F52DFE-D03E-46E6-B5C0-E97283622024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="923925"/>
+          <a:ext cx="1600200" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -855,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -870,221 +943,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="27">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="21"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="21"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="21"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="21"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="21"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="21"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="21"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="21"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="22"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="17" t="e">
+      <c r="D16" s="8" t="e">
         <f>C16-B16</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="8">
         <v>10</v>
       </c>
-      <c r="F16" s="21" t="e">
+      <c r="F16" s="12" t="e">
         <f>E16*D16*24</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="14"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="22"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" ht="15.75">
-      <c r="A18" s="14"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="18" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="19" t="e">
+      <c r="D18" s="10" t="e">
         <f>SUM(D16:D17)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="24" t="e">
+      <c r="F18" s="15" t="e">
         <f>SUM(F16:F17)</f>
         <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1092,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA6A04C-FD9C-4CC0-9A8A-23F665EB3B7C}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1106,179 +1180,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="15.75">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" ht="15.75">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" ht="15.75">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="18" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5" ht="15.75">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" ht="15.75">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" ht="15.75">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" ht="15.75">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
add simple variables insterted vaules to the static variables
</commit_message>
<xml_diff>
--- a/test/templates/simple.xlsx
+++ b/test/templates/simple.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27324"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC14D4D-28CB-491F-8A73-18939993F31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D384B84-F197-4978-88F9-59C871E45835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -489,19 +489,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -929,7 +929,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1119,14 +1119,14 @@
         <v>25</v>
       </c>
       <c r="D16" s="8" t="e">
-        <f>C16-B16</f>
+        <f>ROUND(C16-B16, 4)</f>
         <v>#VALUE!</v>
       </c>
       <c r="E16" s="8">
         <v>10</v>
       </c>
       <c r="F16" s="12" t="e">
-        <f>E16*D16*24</f>
+        <f>ROUND(E16*D16*24, 2)</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>